<commit_message>
Anforderungsartefakte/Prosaanforderungen.xlsx erledigt; kosmetische Aenderungen
</commit_message>
<xml_diff>
--- a/documents/Anforderungsartefakte/Prosaanforderungen.xlsx
+++ b/documents/Anforderungsartefakte/Prosaanforderungen.xlsx
@@ -16,15 +16,77 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>aus pdf-Dokument "Anforderungen Coll@HBRS v2.0" nehmen</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Text</t>
   </si>
   <si>
     <t>Nr.</t>
+  </si>
+  <si>
+    <t>Die persistenten Daten müssen auf einer
+PostgreSQL-DB via JDBC abgespeichert werden.</t>
+  </si>
+  <si>
+    <t>Mit dem Tool SonarQube müssen
+technische Schulden und Bad Code Smells
+Analysiert und visualisiert werden.</t>
+  </si>
+  <si>
+    <t>Die Datenbank muss mit Roundtrip-Tests getestet werden.</t>
+  </si>
+  <si>
+    <t>Die Software muss via SEPP deployed werden.</t>
+  </si>
+  <si>
+    <t>Der externe Zugriff zum deployen der Software via SEPP
+muss via OpenVPN erfolgen.</t>
+  </si>
+  <si>
+    <t>Benachrichtigungen über Software-Fehler sollen per E-Mail gesendet werden.</t>
+  </si>
+  <si>
+    <t>In der Produktivumgebung soll die E-Mail-Benachrichtigung
+im Fehlerfall deaktiviert werden können.</t>
+  </si>
+  <si>
+    <t>Die Datenbankimplementierung soll mit Mockito getestet werden.</t>
+  </si>
+  <si>
+    <t>Der studentische Benutzer soll sich mit seiner Linux-Kennung einloggen können.</t>
+  </si>
+  <si>
+    <t>Der studentische Benutzer soll seinen Account löschen können, um keine weiteren Benachrichtigungen zu bekommen.</t>
+  </si>
+  <si>
+    <t>Unternehmerische Benutzer sollen sich registrieren können.</t>
+  </si>
+  <si>
+    <t>Der studentische Benutzer soll sich ein Profil mit persönlichen Daten und fachlichen Interessen erstellen können.</t>
+  </si>
+  <si>
+    <t>Der studentische Benutzer soll sich nach seinen Qualifikationen, Stärken, befristeten Stellen und Beschäftigungsart filtern können, um passende Stellen zu finden.</t>
+  </si>
+  <si>
+    <t>Der studentische Benutzer soll anhand seiner fachlichen Interessen zu passenden Stellen informiert werden.</t>
+  </si>
+  <si>
+    <t>Der studentische Benutzer soll Unternehmen abonnieren können, um über Neuigkeiten &amp; Stellen informiert zu werden.</t>
+  </si>
+  <si>
+    <t>Der Benutzer benötigt eine passwortgeschützte Anmeldung.</t>
+  </si>
+  <si>
+    <t>Der Benutzer soll eine auf Smartphones angepasste Ansicht des Systems haben.</t>
+  </si>
+  <si>
+    <t>Unternehmerische Benutzer sollen Informationen über ihr Unternehmen bereitstellen können.</t>
+  </si>
+  <si>
+    <t>Unternehmerische Benutzer sollen freie Stellen bereitstellen können.</t>
+  </si>
+  <si>
+    <t>Unternehmerische Benutzer sollen einen Ansprechpartner hinterlegen können.</t>
   </si>
 </sst>
 </file>
@@ -68,9 +130,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -91,16 +156,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>411481</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>395175</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>144781</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>593294</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -117,7 +182,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7940041" y="365761"/>
+          <a:off x="0" y="0"/>
           <a:ext cx="6079694" cy="4168140"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -417,35 +482,189 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.109375" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="84.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -458,6 +677,7 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>